<commit_message>
auto:adding appoitment reminder task to trigger a task 7 days before the appoitment date
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment_reminder.xlsx
+++ b/config/forms/app/appointment_reminder.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="79">
   <si>
     <t>type</t>
   </si>
@@ -206,6 +206,10 @@
   </si>
   <si>
     <t>Client has an upcoming appointment. You may want to follow-up with the client to remind them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noted, delete task from my inbox 
+</t>
   </si>
   <si>
     <t>follow-up</t>
@@ -706,6 +710,7 @@
     <col customWidth="1" min="2" max="2" width="26.88"/>
     <col customWidth="1" min="3" max="3" width="85.38"/>
     <col customWidth="1" min="7" max="7" width="30.88"/>
+    <col customWidth="1" min="9" max="9" width="53.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1342,13 +1347,19 @@
     </row>
     <row r="37">
       <c r="A37" s="21" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>62</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>63</v>
+      </c>
+      <c r="H37" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="21" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="38">
@@ -1356,10 +1367,10 @@
         <v>28</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39">
@@ -1384,7 +1395,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1436,47 +1447,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C2" s="27" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-01-30_15-20</v>
+        <v>2023-01-30_16-29</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F2" s="28"/>
       <c r="G2" s="28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:adding blood draw appoitnment form
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment_reminder.xlsx
+++ b/config/forms/app/appointment_reminder.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="82">
   <si>
     <t>type</t>
   </si>
@@ -84,6 +84,9 @@
     <t>field_date_task_appears</t>
   </si>
   <si>
+    <t>person_comp</t>
+  </si>
+  <si>
     <t>contact</t>
   </si>
   <si>
@@ -168,12 +171,24 @@
     <t>../inputs/field_date_task_appears</t>
   </si>
   <si>
+    <t>person_compl</t>
+  </si>
+  <si>
+    <t>../inputs/person_comp</t>
+  </si>
+  <si>
     <t>appointment_reminder</t>
   </si>
   <si>
     <t>note</t>
   </si>
   <si>
+    <t xml:space="preserve">person_complete </t>
+  </si>
+  <si>
+    <t>**Person who completed this form** ${person_compl}</t>
+  </si>
+  <si>
     <t>**Appointment Type:** ${app_type}</t>
   </si>
   <si>
@@ -195,17 +210,13 @@
     <t>**Notes about this appoitment:** ${notes}</t>
   </si>
   <si>
-    <t>date_task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Date Task Appears :** ${date_task_appears}
+    <t xml:space="preserve">upcoming </t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Reminder! Client has an appointment soon.**
+ **.** Noted, I will follow-up as needed. Delete this Task 
+ **.** Keep this reminder in my Task List
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">upcoming </t>
-  </si>
-  <si>
-    <t>Client has an upcoming appointment. You may want to follow-up with the client to remind them.</t>
   </si>
   <si>
     <t xml:space="preserve">Noted, delete task from my inbox 
@@ -888,15 +899,13 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="C10" s="7"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -906,19 +915,17 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -927,17 +934,17 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -947,10 +954,10 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>12</v>
@@ -967,10 +974,10 @@
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>12</v>
@@ -987,7 +994,7 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>31</v>
@@ -1006,27 +1013,31 @@
       <c r="J15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="12" t="s">
+      <c r="A16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>12</v>
@@ -1038,29 +1049,27 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>33</v>
+      <c r="A18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>12</v>
@@ -1074,20 +1083,26 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -1099,7 +1114,7 @@
     </row>
     <row r="22">
       <c r="A22" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
@@ -1111,7 +1126,7 @@
     </row>
     <row r="23">
       <c r="A23" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
@@ -1125,62 +1140,56 @@
       <c r="A24" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="13" t="s">
-        <v>37</v>
-      </c>
+      <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>12</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="16" t="s">
-        <v>42</v>
+      <c r="G26" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27">
       <c r="A27" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>12</v>
@@ -1189,16 +1198,16 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H27" s="2"/>
     </row>
     <row r="28">
       <c r="A28" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>12</v>
@@ -1207,16 +1216,16 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>12</v>
@@ -1225,16 +1234,16 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H29" s="2"/>
     </row>
     <row r="30">
       <c r="A30" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>12</v>
@@ -1243,71 +1252,75 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="19" t="s">
+      <c r="C31" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
     <row r="32">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>53</v>
+      <c r="C32" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="G32" s="16" t="s">
+        <v>53</v>
+      </c>
       <c r="H32" s="2"/>
     </row>
     <row r="33">
-      <c r="A33" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="20" t="s">
+      <c r="A33" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="20" t="s">
-        <v>55</v>
+      <c r="C33" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34">
-      <c r="A34" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="20" t="s">
+      <c r="A34" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>56</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="18"/>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -1315,13 +1328,13 @@
     </row>
     <row r="35">
       <c r="A35" s="20" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B35" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="20" t="s">
         <v>58</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>59</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1331,13 +1344,13 @@
     </row>
     <row r="36">
       <c r="A36" s="20" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B36" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>60</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>61</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1346,36 +1359,68 @@
       <c r="H36" s="2"/>
     </row>
     <row r="37">
-      <c r="A37" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="21" t="s">
+      <c r="A37" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="D37" s="18"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="H37" s="21" t="b">
+      <c r="C38" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H39" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="I37" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="14" t="s">
-        <v>34</v>
+      <c r="I39" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1395,7 +1440,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1447,47 +1492,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="26" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C2" s="27" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-01-30_16-29</v>
+        <v>2023-08-20_15-29</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F2" s="28"/>
       <c r="G2" s="28" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:adding changes and edits in the blood draw appointment
</commit_message>
<xml_diff>
--- a/config/forms/app/appointment_reminder.xlsx
+++ b/config/forms/app/appointment_reminder.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
   <si>
     <t>type</t>
   </si>
@@ -192,12 +192,6 @@
     <t>**Appointment Type:** ${app_type}</t>
   </si>
   <si>
-    <t>blood_draw</t>
-  </si>
-  <si>
-    <t>**Blood draw type:** ${blood_draw_type}</t>
-  </si>
-  <si>
     <t>appointment_date</t>
   </si>
   <si>
@@ -210,12 +204,13 @@
     <t>**Notes about this appoitment:** ${notes}</t>
   </si>
   <si>
+    <t>select_one soon</t>
+  </si>
+  <si>
     <t xml:space="preserve">upcoming </t>
   </si>
   <si>
-    <t xml:space="preserve">**Reminder! Client has an appointment soon.**
- **.** Noted, I will follow-up as needed. Delete this Task 
- **.** Keep this reminder in my Task List
+    <t xml:space="preserve">Reminder! Client has an appointment soon.
 </t>
   </si>
   <si>
@@ -247,6 +242,21 @@
   </si>
   <si>
     <t>list_name</t>
+  </si>
+  <si>
+    <t>soon</t>
+  </si>
+  <si>
+    <t>soon_noted</t>
+  </si>
+  <si>
+    <t>Noted, I will follow-up as needed. Delete this Task</t>
+  </si>
+  <si>
+    <t>soon_keep</t>
+  </si>
+  <si>
+    <t>Keep this reminder in my Task List</t>
   </si>
   <si>
     <t>form_title</t>
@@ -1352,7 +1362,7 @@
       <c r="C36" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -1368,58 +1378,42 @@
       <c r="C37" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="18"/>
+      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="20" t="s">
+      <c r="A38" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="C38" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="H38" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="21" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="21" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H39" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" s="21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="14" t="s">
+      <c r="A40" s="14" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1437,10 +1431,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="37.13"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1472,6 +1469,28 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
+    <row r="2">
+      <c r="A2" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1492,47 +1511,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="23" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="26" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="27" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-08-20_15-29</v>
+        <v>2023-08-23_22-29</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F2" s="28"/>
       <c r="G2" s="28" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>